<commit_message>
Changed equity return script for automotive data set
</commit_message>
<xml_diff>
--- a/data/Series_Selection/selected_series.xlsx
+++ b/data/Series_Selection/selected_series.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="18420" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="18420" tabRatio="510" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Insurance" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="124">
   <si>
     <t>Insurance</t>
   </si>
@@ -378,6 +378,30 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>data.set = "automotive"</t>
+  </si>
+  <si>
+    <t>zero.cutoff &lt;- 0.0005 # returns / differences smaller than this threshold value are considered to be zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  #empirical_cdf &lt;- kcde(unlist(X), h = bw_parameter)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  empirical_cdf &lt;- kcde(X, h = bw_parameter)</t>
+  </si>
+  <si>
+    <t>user.bw = 0.0005 # 0.0003</t>
+  </si>
+  <si>
+    <t>Volkswagen</t>
+  </si>
+  <si>
+    <t>bw</t>
+  </si>
+  <si>
+    <t>binw</t>
   </si>
 </sst>
 </file>
@@ -684,6 +708,87 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>397811</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6276975" y="247650"/>
+          <a:ext cx="7541561" cy="7077075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>133351</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>255972</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>438151</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>103998</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15992476" y="255972"/>
+          <a:ext cx="7620000" cy="7048926"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1568,293 +1673,624 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A273"/>
+  <dimension ref="A1:S206"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P57" sqref="P57"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC61" sqref="AC61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="73.28515625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="5" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="7" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="9" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="10" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="12" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="15" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="16" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="21" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="22" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="24" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="25" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="27" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="28" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="32" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="88" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="90" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="91" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="97" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="98" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="99" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="100" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="101" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="102" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="103" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="104" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="105" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="106" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="107" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="108" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="109" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="110" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="111" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="112" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="113" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="114" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="115" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="116" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="117" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="118" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="119" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="120" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="121" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="122" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="123" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="124" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="125" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="126" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="127" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="128" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="129" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="130" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="131" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="132" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="133" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="134" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="135" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="136" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="137" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="138" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="139" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="140" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="141" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="142" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="143" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="144" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="145" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="146" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="147" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="148" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="149" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="150" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="151" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="152" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="153" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="154" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="155" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="156" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="157" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="158" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="159" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="160" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="161" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="162" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="163" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="164" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="165" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="166" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="167" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="168" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="169" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="170" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="171" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="172" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="173" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="174" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="175" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="176" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="177" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="178" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="179" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="180" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="181" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="182" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="183" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="184" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="185" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="186" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="187" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="188" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="189" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="190" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="191" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="192" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="193" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="194" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="195" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="196" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="197" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="198" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="199" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="200" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="201" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="202" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="203" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="204" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="205" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="206" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="207" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="208" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="209" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="210" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="211" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="212" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="213" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="214" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="215" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="216" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="217" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="218" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="219" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="220" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="221" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="222" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="223" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="224" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="225" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="226" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="227" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="228" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="229" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="230" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="231" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="232" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="233" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="234" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="235" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="236" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="237" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="238" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="239" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="240" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="241" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="242" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="243" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="244" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="245" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="246" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="247" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="248" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="249" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="250" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="251" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="252" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="253" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="254" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="255" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="256" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="257" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="258" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="259" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="260" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="261" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="262" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="263" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="264" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="265" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="266" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="267" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="268" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="269" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="270" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="271" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="272" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="273" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="1:19" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R6" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="S6" s="1">
+        <v>3.5E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="R7" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="198" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A198" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="199" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A199" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="201" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A201" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="202" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A202" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="203" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A203" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A204" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A205" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A206" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>